<commit_message>
update the BO: search_space vs fixed_space
</commit_message>
<xml_diff>
--- a/04_Model_Saved/NN_full_RepeatedKFold_v3_BO_test/MultiTaskModel_NiCrCoVFe_KW99_wt_pct_ML.xlsx
+++ b/04_Model_Saved/NN_full_RepeatedKFold_v3_BO_test/MultiTaskModel_NiCrCoVFe_KW99_wt_pct_ML.xlsx
@@ -505,16 +505,16 @@
         <v>10.27148578895017</v>
       </c>
       <c r="G2" t="n">
-        <v>196.5256652832031</v>
+        <v>195.2227325439453</v>
       </c>
       <c r="H2" t="n">
-        <v>52.06587982177734</v>
+        <v>51.67490386962891</v>
       </c>
       <c r="I2" t="n">
-        <v>480.3932800292969</v>
+        <v>482.7013549804688</v>
       </c>
       <c r="J2" t="n">
-        <v>106.7970275878906</v>
+        <v>99.68337249755859</v>
       </c>
     </row>
     <row r="3">
@@ -537,16 +537,16 @@
         <v>10.49540628405087</v>
       </c>
       <c r="G3" t="n">
-        <v>202.4033203125</v>
+        <v>200.2395629882812</v>
       </c>
       <c r="H3" t="n">
-        <v>48.53744125366211</v>
+        <v>47.55746078491211</v>
       </c>
       <c r="I3" t="n">
-        <v>506.9461975097656</v>
+        <v>503.849853515625</v>
       </c>
       <c r="J3" t="n">
-        <v>118.2903137207031</v>
+        <v>120.1978302001953</v>
       </c>
     </row>
     <row r="4">
@@ -569,16 +569,16 @@
         <v>11.11292799977388</v>
       </c>
       <c r="G4" t="n">
-        <v>207.6016235351562</v>
+        <v>206.0742034912109</v>
       </c>
       <c r="H4" t="n">
-        <v>48.72306060791016</v>
+        <v>48.16543960571289</v>
       </c>
       <c r="I4" t="n">
-        <v>507.2357788085938</v>
+        <v>513.5458984375</v>
       </c>
       <c r="J4" t="n">
-        <v>123.5246276855469</v>
+        <v>124.2968521118164</v>
       </c>
     </row>
     <row r="5">
@@ -601,16 +601,16 @@
         <v>11.33579528302992</v>
       </c>
       <c r="G5" t="n">
-        <v>213.3286590576172</v>
+        <v>213.8444671630859</v>
       </c>
       <c r="H5" t="n">
-        <v>48.412841796875</v>
+        <v>50.01402282714844</v>
       </c>
       <c r="I5" t="n">
-        <v>497.05078125</v>
+        <v>489.4606323242188</v>
       </c>
       <c r="J5" t="n">
-        <v>136.0558624267578</v>
+        <v>131.1631469726562</v>
       </c>
     </row>
     <row r="6">
@@ -633,16 +633,16 @@
         <v>11.53221857575777</v>
       </c>
       <c r="G6" t="n">
-        <v>216.4931793212891</v>
+        <v>216.2987823486328</v>
       </c>
       <c r="H6" t="n">
-        <v>48.52336883544922</v>
+        <v>49.52398300170898</v>
       </c>
       <c r="I6" t="n">
-        <v>435.5796203613281</v>
+        <v>436.9855346679688</v>
       </c>
       <c r="J6" t="n">
-        <v>155.2930297851562</v>
+        <v>155.8653259277344</v>
       </c>
     </row>
     <row r="7">
@@ -665,16 +665,16 @@
         <v>11.73836346032553</v>
       </c>
       <c r="G7" t="n">
-        <v>174.3065338134766</v>
+        <v>176.4867095947266</v>
       </c>
       <c r="H7" t="n">
-        <v>53.14573669433594</v>
+        <v>54.24579238891602</v>
       </c>
       <c r="I7" t="n">
-        <v>381.8974609375</v>
+        <v>385.7624206542969</v>
       </c>
       <c r="J7" t="n">
-        <v>83.40523529052734</v>
+        <v>88.20526885986328</v>
       </c>
     </row>
     <row r="8">
@@ -697,16 +697,16 @@
         <v>12.47588443056982</v>
       </c>
       <c r="G8" t="n">
-        <v>184.0388946533203</v>
+        <v>186.3274841308594</v>
       </c>
       <c r="H8" t="n">
-        <v>52.79661560058594</v>
+        <v>55.65920257568359</v>
       </c>
       <c r="I8" t="n">
-        <v>410.9967956542969</v>
+        <v>411.7225341796875</v>
       </c>
       <c r="J8" t="n">
-        <v>89.63048553466797</v>
+        <v>91.81758117675781</v>
       </c>
     </row>
     <row r="9">
@@ -729,16 +729,16 @@
         <v>13.31360035996819</v>
       </c>
       <c r="G9" t="n">
-        <v>196.4605712890625</v>
+        <v>192.0022583007812</v>
       </c>
       <c r="H9" t="n">
-        <v>52.95595169067383</v>
+        <v>52.12316131591797</v>
       </c>
       <c r="I9" t="n">
-        <v>431.9489440917969</v>
+        <v>438.3903198242188</v>
       </c>
       <c r="J9" t="n">
-        <v>93.29929351806641</v>
+        <v>98.35660552978516</v>
       </c>
     </row>
     <row r="10">
@@ -761,16 +761,16 @@
         <v>14.04586286313179</v>
       </c>
       <c r="G10" t="n">
-        <v>201.8445281982422</v>
+        <v>199.0718231201172</v>
       </c>
       <c r="H10" t="n">
-        <v>49.16138458251953</v>
+        <v>47.32728576660156</v>
       </c>
       <c r="I10" t="n">
-        <v>447.5711364746094</v>
+        <v>449.5156860351562</v>
       </c>
       <c r="J10" t="n">
-        <v>103.2507553100586</v>
+        <v>102.3488235473633</v>
       </c>
     </row>
     <row r="11">
@@ -793,16 +793,16 @@
         <v>14.78596965177877</v>
       </c>
       <c r="G11" t="n">
-        <v>208.4149627685547</v>
+        <v>209.9117431640625</v>
       </c>
       <c r="H11" t="n">
-        <v>48.00620651245117</v>
+        <v>46.67269515991211</v>
       </c>
       <c r="I11" t="n">
-        <v>448.8161010742188</v>
+        <v>450.6067810058594</v>
       </c>
       <c r="J11" t="n">
-        <v>119.5340270996094</v>
+        <v>114.9870986938477</v>
       </c>
     </row>
     <row r="12">
@@ -825,16 +825,16 @@
         <v>14.60750023008277</v>
       </c>
       <c r="G12" t="n">
-        <v>212.5779571533203</v>
+        <v>214.5973968505859</v>
       </c>
       <c r="H12" t="n">
-        <v>48.53993988037109</v>
+        <v>48.46996307373047</v>
       </c>
       <c r="I12" t="n">
-        <v>419.3351440429688</v>
+        <v>416.9954833984375</v>
       </c>
       <c r="J12" t="n">
-        <v>145.3392181396484</v>
+        <v>151.6266479492188</v>
       </c>
     </row>
     <row r="13">
@@ -857,16 +857,16 @@
         <v>13.93632017907879</v>
       </c>
       <c r="G13" t="n">
-        <v>217.4632415771484</v>
+        <v>216.9892425537109</v>
       </c>
       <c r="H13" t="n">
-        <v>49.02243804931641</v>
+        <v>47.44356155395508</v>
       </c>
       <c r="I13" t="n">
-        <v>351.4627685546875</v>
+        <v>358.7764892578125</v>
       </c>
       <c r="J13" t="n">
-        <v>163.1253967285156</v>
+        <v>155.7240600585938</v>
       </c>
     </row>
     <row r="14">
@@ -889,16 +889,16 @@
         <v>13.2060787967079</v>
       </c>
       <c r="G14" t="n">
-        <v>162.9321136474609</v>
+        <v>161.88037109375</v>
       </c>
       <c r="H14" t="n">
-        <v>57.33430862426758</v>
+        <v>56.76521682739258</v>
       </c>
       <c r="I14" t="n">
-        <v>251.0800476074219</v>
+        <v>253.1082611083984</v>
       </c>
       <c r="J14" t="n">
-        <v>100.6155624389648</v>
+        <v>101.2411575317383</v>
       </c>
     </row>
     <row r="15">
@@ -921,16 +921,16 @@
         <v>14.43724685121477</v>
       </c>
       <c r="G15" t="n">
-        <v>173.6306610107422</v>
+        <v>172.6675109863281</v>
       </c>
       <c r="H15" t="n">
-        <v>57.75284957885742</v>
+        <v>56.87653350830078</v>
       </c>
       <c r="I15" t="n">
-        <v>306.8633728027344</v>
+        <v>310.6955871582031</v>
       </c>
       <c r="J15" t="n">
-        <v>96.7650146484375</v>
+        <v>99.13153839111328</v>
       </c>
     </row>
     <row r="16">
@@ -953,16 +953,16 @@
         <v>15.77509757365795</v>
       </c>
       <c r="G16" t="n">
-        <v>181.034912109375</v>
+        <v>183.4707946777344</v>
       </c>
       <c r="H16" t="n">
-        <v>56.13068771362305</v>
+        <v>55.19968795776367</v>
       </c>
       <c r="I16" t="n">
-        <v>351.9544982910156</v>
+        <v>349.7698059082031</v>
       </c>
       <c r="J16" t="n">
-        <v>92.00080108642578</v>
+        <v>91.99127197265625</v>
       </c>
     </row>
     <row r="17">
@@ -985,16 +985,16 @@
         <v>17.01643502058164</v>
       </c>
       <c r="G17" t="n">
-        <v>191.7245788574219</v>
+        <v>189.1093597412109</v>
       </c>
       <c r="H17" t="n">
-        <v>53.76506805419922</v>
+        <v>53.9105110168457</v>
       </c>
       <c r="I17" t="n">
-        <v>396.2289733886719</v>
+        <v>396.6742553710938</v>
       </c>
       <c r="J17" t="n">
-        <v>95.50647735595703</v>
+        <v>94.58293914794922</v>
       </c>
     </row>
     <row r="18">
@@ -1017,16 +1017,16 @@
         <v>17.57324774662381</v>
       </c>
       <c r="G18" t="n">
-        <v>196.9173889160156</v>
+        <v>193.5535125732422</v>
       </c>
       <c r="H18" t="n">
-        <v>51.15447998046875</v>
+        <v>49.10778045654297</v>
       </c>
       <c r="I18" t="n">
-        <v>406.003173828125</v>
+        <v>408.5403747558594</v>
       </c>
       <c r="J18" t="n">
-        <v>98.87155151367188</v>
+        <v>102.0366592407227</v>
       </c>
     </row>
     <row r="19">
@@ -1049,16 +1049,16 @@
         <v>18.2282289394109</v>
       </c>
       <c r="G19" t="n">
-        <v>204.9086303710938</v>
+        <v>204.7497863769531</v>
       </c>
       <c r="H19" t="n">
-        <v>49.24051666259766</v>
+        <v>48.77395629882812</v>
       </c>
       <c r="I19" t="n">
-        <v>424.8413696289062</v>
+        <v>421.1508178710938</v>
       </c>
       <c r="J19" t="n">
-        <v>118.5129547119141</v>
+        <v>113.3203811645508</v>
       </c>
     </row>
     <row r="20">
@@ -1081,16 +1081,16 @@
         <v>18.05168677518481</v>
       </c>
       <c r="G20" t="n">
-        <v>212.4664001464844</v>
+        <v>212.5441741943359</v>
       </c>
       <c r="H20" t="n">
-        <v>49.24223327636719</v>
+        <v>48.45927810668945</v>
       </c>
       <c r="I20" t="n">
-        <v>406.3514709472656</v>
+        <v>403.0552978515625</v>
       </c>
       <c r="J20" t="n">
-        <v>135.9393005371094</v>
+        <v>134.3570556640625</v>
       </c>
     </row>
     <row r="21">
@@ -1113,16 +1113,16 @@
         <v>17.30316829702608</v>
       </c>
       <c r="G21" t="n">
-        <v>219.1393432617188</v>
+        <v>221.4381713867188</v>
       </c>
       <c r="H21" t="n">
-        <v>50.23594665527344</v>
+        <v>51.19360733032227</v>
       </c>
       <c r="I21" t="n">
-        <v>367.5068054199219</v>
+        <v>370.1768493652344</v>
       </c>
       <c r="J21" t="n">
-        <v>161.6315002441406</v>
+        <v>166.2844848632812</v>
       </c>
     </row>
     <row r="22">
@@ -1145,16 +1145,16 @@
         <v>15.87142913305469</v>
       </c>
       <c r="G22" t="n">
-        <v>274.2776184082031</v>
+        <v>274.8809509277344</v>
       </c>
       <c r="H22" t="n">
-        <v>92.11920928955078</v>
+        <v>92.05734252929688</v>
       </c>
       <c r="I22" t="n">
-        <v>308.2761840820312</v>
+        <v>306.1294250488281</v>
       </c>
       <c r="J22" t="n">
-        <v>180.3496551513672</v>
+        <v>186.4326934814453</v>
       </c>
     </row>
     <row r="23">
@@ -1177,16 +1177,16 @@
         <v>16.2842163689804</v>
       </c>
       <c r="G23" t="n">
-        <v>157.2698364257812</v>
+        <v>157.1050262451172</v>
       </c>
       <c r="H23" t="n">
-        <v>54.64023971557617</v>
+        <v>54.61679077148438</v>
       </c>
       <c r="I23" t="n">
-        <v>211.4840087890625</v>
+        <v>205.2504577636719</v>
       </c>
       <c r="J23" t="n">
-        <v>111.4083023071289</v>
+        <v>108.8575897216797</v>
       </c>
     </row>
     <row r="24">
@@ -1209,16 +1209,16 @@
         <v>17.99859633271077</v>
       </c>
       <c r="G24" t="n">
-        <v>170.9324645996094</v>
+        <v>166.8280792236328</v>
       </c>
       <c r="H24" t="n">
-        <v>59.41715240478516</v>
+        <v>53.18321990966797</v>
       </c>
       <c r="I24" t="n">
-        <v>254.4470520019531</v>
+        <v>254.1157836914062</v>
       </c>
       <c r="J24" t="n">
-        <v>102.835205078125</v>
+        <v>103.4831466674805</v>
       </c>
     </row>
     <row r="25">
@@ -1241,16 +1241,16 @@
         <v>19.53665474474453</v>
       </c>
       <c r="G25" t="n">
-        <v>175.4058380126953</v>
+        <v>175.8715057373047</v>
       </c>
       <c r="H25" t="n">
-        <v>57.06556701660156</v>
+        <v>54.89497375488281</v>
       </c>
       <c r="I25" t="n">
-        <v>298.1505737304688</v>
+        <v>297.2965087890625</v>
       </c>
       <c r="J25" t="n">
-        <v>100.1256256103516</v>
+        <v>102.2621078491211</v>
       </c>
     </row>
     <row r="26">
@@ -1273,16 +1273,16 @@
         <v>21.18080958029204</v>
       </c>
       <c r="G26" t="n">
-        <v>184.573974609375</v>
+        <v>184.5228576660156</v>
       </c>
       <c r="H26" t="n">
-        <v>53.67688369750977</v>
+        <v>53.16211700439453</v>
       </c>
       <c r="I26" t="n">
-        <v>344.0014953613281</v>
+        <v>346.1135559082031</v>
       </c>
       <c r="J26" t="n">
-        <v>97.35845947265625</v>
+        <v>104.3116683959961</v>
       </c>
     </row>
     <row r="27">
@@ -1305,16 +1305,16 @@
         <v>22.36133238808863</v>
       </c>
       <c r="G27" t="n">
-        <v>196.0658264160156</v>
+        <v>195.1513671875</v>
       </c>
       <c r="H27" t="n">
-        <v>53.56443023681641</v>
+        <v>53.19629669189453</v>
       </c>
       <c r="I27" t="n">
-        <v>387.2424011230469</v>
+        <v>383.5699768066406</v>
       </c>
       <c r="J27" t="n">
-        <v>107.8214645385742</v>
+        <v>105.8611068725586</v>
       </c>
     </row>
     <row r="28">
@@ -1337,16 +1337,16 @@
         <v>22.25528267810615</v>
       </c>
       <c r="G28" t="n">
-        <v>201.9727172851562</v>
+        <v>202.7328796386719</v>
       </c>
       <c r="H28" t="n">
-        <v>52.50704956054688</v>
+        <v>52.11050796508789</v>
       </c>
       <c r="I28" t="n">
-        <v>404.7824096679688</v>
+        <v>400.4265747070312</v>
       </c>
       <c r="J28" t="n">
-        <v>113.7992553710938</v>
+        <v>113.4826202392578</v>
       </c>
     </row>
     <row r="29">
@@ -1369,16 +1369,16 @@
         <v>22.11853696692908</v>
       </c>
       <c r="G29" t="n">
-        <v>218.0038146972656</v>
+        <v>215.2844848632812</v>
       </c>
       <c r="H29" t="n">
-        <v>57.47426986694336</v>
+        <v>55.07153701782227</v>
       </c>
       <c r="I29" t="n">
-        <v>407.0451049804688</v>
+        <v>395.2782287597656</v>
       </c>
       <c r="J29" t="n">
-        <v>143.2666015625</v>
+        <v>142.4566345214844</v>
       </c>
     </row>
     <row r="30">
@@ -1401,16 +1401,16 @@
         <v>21.13587239531939</v>
       </c>
       <c r="G30" t="n">
-        <v>241.1434326171875</v>
+        <v>242.7356262207031</v>
       </c>
       <c r="H30" t="n">
-        <v>66.76734924316406</v>
+        <v>68.04347229003906</v>
       </c>
       <c r="I30" t="n">
-        <v>379.5373229980469</v>
+        <v>382.4942016601562</v>
       </c>
       <c r="J30" t="n">
-        <v>167.7958526611328</v>
+        <v>162.1541748046875</v>
       </c>
     </row>
     <row r="31">
@@ -1433,16 +1433,16 @@
         <v>19.80061812897557</v>
       </c>
       <c r="G31" t="n">
-        <v>320.9665222167969</v>
+        <v>324.3143615722656</v>
       </c>
       <c r="H31" t="n">
-        <v>117.7856903076172</v>
+        <v>117.8579940795898</v>
       </c>
       <c r="I31" t="n">
-        <v>332.4823303222656</v>
+        <v>335.6470947265625</v>
       </c>
       <c r="J31" t="n">
-        <v>197.7228393554688</v>
+        <v>185.4528503417969</v>
       </c>
     </row>
     <row r="32">
@@ -1465,16 +1465,16 @@
         <v>20.55168297688286</v>
       </c>
       <c r="G32" t="n">
-        <v>157.4930725097656</v>
+        <v>158.0298156738281</v>
       </c>
       <c r="H32" t="n">
-        <v>55.82131195068359</v>
+        <v>56.26475143432617</v>
       </c>
       <c r="I32" t="n">
-        <v>170.9448394775391</v>
+        <v>173.8154449462891</v>
       </c>
       <c r="J32" t="n">
-        <v>118.7128143310547</v>
+        <v>121.2768630981445</v>
       </c>
     </row>
     <row r="33">
@@ -1497,16 +1497,16 @@
         <v>22.96934284445093</v>
       </c>
       <c r="G33" t="n">
-        <v>166.2661895751953</v>
+        <v>168.2164001464844</v>
       </c>
       <c r="H33" t="n">
-        <v>55.26973724365234</v>
+        <v>58.11928939819336</v>
       </c>
       <c r="I33" t="n">
-        <v>217.0733795166016</v>
+        <v>217.3078765869141</v>
       </c>
       <c r="J33" t="n">
-        <v>111.3954086303711</v>
+        <v>115.5890426635742</v>
       </c>
     </row>
     <row r="34">
@@ -1529,16 +1529,16 @@
         <v>24.40915250803127</v>
       </c>
       <c r="G34" t="n">
-        <v>171.4288482666016</v>
+        <v>172.0601501464844</v>
       </c>
       <c r="H34" t="n">
-        <v>53.87882614135742</v>
+        <v>54.41344833374023</v>
       </c>
       <c r="I34" t="n">
-        <v>260.09912109375</v>
+        <v>254.8300323486328</v>
       </c>
       <c r="J34" t="n">
-        <v>105.767333984375</v>
+        <v>105.8871459960938</v>
       </c>
     </row>
     <row r="35">
@@ -1561,16 +1561,16 @@
         <v>26.0811880993595</v>
       </c>
       <c r="G35" t="n">
-        <v>183.1297454833984</v>
+        <v>181.7398376464844</v>
       </c>
       <c r="H35" t="n">
-        <v>53.66178894042969</v>
+        <v>55.25783920288086</v>
       </c>
       <c r="I35" t="n">
-        <v>310.2444763183594</v>
+        <v>306.9314575195312</v>
       </c>
       <c r="J35" t="n">
-        <v>107.9306488037109</v>
+        <v>109.9947280883789</v>
       </c>
     </row>
     <row r="36">
@@ -1593,16 +1593,16 @@
         <v>26.87614780904968</v>
       </c>
       <c r="G36" t="n">
-        <v>190.8394317626953</v>
+        <v>194.2947845458984</v>
       </c>
       <c r="H36" t="n">
-        <v>53.10575866699219</v>
+        <v>54.4129753112793</v>
       </c>
       <c r="I36" t="n">
-        <v>347.4703979492188</v>
+        <v>346.4244384765625</v>
       </c>
       <c r="J36" t="n">
-        <v>109.5463943481445</v>
+        <v>106.2180557250977</v>
       </c>
     </row>
     <row r="37">
@@ -1625,16 +1625,16 @@
         <v>27.16629873490772</v>
       </c>
       <c r="G37" t="n">
-        <v>200.5313873291016</v>
+        <v>203.4267272949219</v>
       </c>
       <c r="H37" t="n">
-        <v>52.34231948852539</v>
+        <v>56.04669952392578</v>
       </c>
       <c r="I37" t="n">
-        <v>382.5782775878906</v>
+        <v>379.5975036621094</v>
       </c>
       <c r="J37" t="n">
-        <v>122.8509216308594</v>
+        <v>122.7681198120117</v>
       </c>
     </row>
     <row r="38">
@@ -1657,16 +1657,16 @@
         <v>27.25598473560972</v>
       </c>
       <c r="G38" t="n">
-        <v>217.5477142333984</v>
+        <v>217.6856384277344</v>
       </c>
       <c r="H38" t="n">
-        <v>56.69277191162109</v>
+        <v>58.51677703857422</v>
       </c>
       <c r="I38" t="n">
-        <v>396.5762329101562</v>
+        <v>393.49951171875</v>
       </c>
       <c r="J38" t="n">
-        <v>146.4638671875</v>
+        <v>134.5015716552734</v>
       </c>
     </row>
     <row r="39">
@@ -1689,16 +1689,16 @@
         <v>26.04628332899345</v>
       </c>
       <c r="G39" t="n">
-        <v>251.389892578125</v>
+        <v>250.5496063232422</v>
       </c>
       <c r="H39" t="n">
-        <v>77.44590759277344</v>
+        <v>78.32755279541016</v>
       </c>
       <c r="I39" t="n">
-        <v>387.6821594238281</v>
+        <v>377.0298156738281</v>
       </c>
       <c r="J39" t="n">
-        <v>180.3702087402344</v>
+        <v>168.8560485839844</v>
       </c>
     </row>
     <row r="40">
@@ -1721,16 +1721,16 @@
         <v>23.96978635149335</v>
       </c>
       <c r="G40" t="n">
-        <v>338.9738159179688</v>
+        <v>346.5497436523438</v>
       </c>
       <c r="H40" t="n">
-        <v>115.8012161254883</v>
+        <v>117.4175796508789</v>
       </c>
       <c r="I40" t="n">
-        <v>353.9007263183594</v>
+        <v>353.0171508789062</v>
       </c>
       <c r="J40" t="n">
-        <v>200.5362091064453</v>
+        <v>198.1498260498047</v>
       </c>
     </row>
     <row r="41">
@@ -1753,16 +1753,16 @@
         <v>25.6116837653232</v>
       </c>
       <c r="G41" t="n">
-        <v>155.5841674804688</v>
+        <v>157.2850646972656</v>
       </c>
       <c r="H41" t="n">
-        <v>52.93328857421875</v>
+        <v>55.76660919189453</v>
       </c>
       <c r="I41" t="n">
-        <v>141.9791259765625</v>
+        <v>139.6143035888672</v>
       </c>
       <c r="J41" t="n">
-        <v>134.6216278076172</v>
+        <v>128.1584777832031</v>
       </c>
     </row>
     <row r="42">
@@ -1785,16 +1785,16 @@
         <v>28.41067839248494</v>
       </c>
       <c r="G42" t="n">
-        <v>165.8793029785156</v>
+        <v>164.2428741455078</v>
       </c>
       <c r="H42" t="n">
-        <v>52.96996688842773</v>
+        <v>54.67495346069336</v>
       </c>
       <c r="I42" t="n">
-        <v>172.3889770507812</v>
+        <v>169.7189483642578</v>
       </c>
       <c r="J42" t="n">
-        <v>119.9296493530273</v>
+        <v>116.6828460693359</v>
       </c>
     </row>
     <row r="43">
@@ -1817,16 +1817,16 @@
         <v>30.68040031937237</v>
       </c>
       <c r="G43" t="n">
-        <v>173.8209838867188</v>
+        <v>171.1742401123047</v>
       </c>
       <c r="H43" t="n">
-        <v>55.01861953735352</v>
+        <v>53.7847785949707</v>
       </c>
       <c r="I43" t="n">
-        <v>215.5758209228516</v>
+        <v>216.7077484130859</v>
       </c>
       <c r="J43" t="n">
-        <v>113.8909454345703</v>
+        <v>113.1384811401367</v>
       </c>
     </row>
     <row r="44">
@@ -1849,16 +1849,16 @@
         <v>32.34762367758118</v>
       </c>
       <c r="G44" t="n">
-        <v>182.4794006347656</v>
+        <v>182.2672119140625</v>
       </c>
       <c r="H44" t="n">
-        <v>54.563720703125</v>
+        <v>54.15227890014648</v>
       </c>
       <c r="I44" t="n">
-        <v>271.4873352050781</v>
+        <v>263.5171203613281</v>
       </c>
       <c r="J44" t="n">
-        <v>115.8154220581055</v>
+        <v>116.8299026489258</v>
       </c>
     </row>
     <row r="45">
@@ -1881,16 +1881,16 @@
         <v>33.26712421235609</v>
       </c>
       <c r="G45" t="n">
-        <v>187.9643096923828</v>
+        <v>192.22021484375</v>
       </c>
       <c r="H45" t="n">
-        <v>54.44453430175781</v>
+        <v>54.14269256591797</v>
       </c>
       <c r="I45" t="n">
-        <v>318.1514587402344</v>
+        <v>321.3756103515625</v>
       </c>
       <c r="J45" t="n">
-        <v>118.3914413452148</v>
+        <v>117.304069519043</v>
       </c>
     </row>
     <row r="46">
@@ -1913,16 +1913,16 @@
         <v>33.39925272231932</v>
       </c>
       <c r="G46" t="n">
-        <v>205.8799896240234</v>
+        <v>204.1011352539062</v>
       </c>
       <c r="H46" t="n">
-        <v>55.51567840576172</v>
+        <v>56.34929656982422</v>
       </c>
       <c r="I46" t="n">
-        <v>368.1354370117188</v>
+        <v>379.4385070800781</v>
       </c>
       <c r="J46" t="n">
-        <v>123.9568634033203</v>
+        <v>134.6839447021484</v>
       </c>
     </row>
     <row r="47">
@@ -1945,16 +1945,16 @@
         <v>32.83385481517335</v>
       </c>
       <c r="G47" t="n">
-        <v>220.0856018066406</v>
+        <v>218.7140350341797</v>
       </c>
       <c r="H47" t="n">
-        <v>60.26463317871094</v>
+        <v>60.0420036315918</v>
       </c>
       <c r="I47" t="n">
-        <v>395.963623046875</v>
+        <v>400.7065734863281</v>
       </c>
       <c r="J47" t="n">
-        <v>154.9861755371094</v>
+        <v>150.1612548828125</v>
       </c>
     </row>
     <row r="48">
@@ -1977,16 +1977,16 @@
         <v>31.22587875804939</v>
       </c>
       <c r="G48" t="n">
-        <v>266.0925903320312</v>
+        <v>267.2758483886719</v>
       </c>
       <c r="H48" t="n">
-        <v>83.48360443115234</v>
+        <v>83.80287170410156</v>
       </c>
       <c r="I48" t="n">
-        <v>398.7019653320312</v>
+        <v>400.8147888183594</v>
       </c>
       <c r="J48" t="n">
-        <v>206.7093658447266</v>
+        <v>199.1689910888672</v>
       </c>
     </row>
     <row r="49">
@@ -2009,16 +2009,16 @@
         <v>28.00050845971687</v>
       </c>
       <c r="G49" t="n">
-        <v>344.2675476074219</v>
+        <v>346.7965698242188</v>
       </c>
       <c r="H49" t="n">
-        <v>115.1764297485352</v>
+        <v>122.2679672241211</v>
       </c>
       <c r="I49" t="n">
-        <v>375.5013122558594</v>
+        <v>377.3677062988281</v>
       </c>
       <c r="J49" t="n">
-        <v>208.1877136230469</v>
+        <v>218.2830505371094</v>
       </c>
     </row>
     <row r="50">
@@ -2041,16 +2041,16 @@
         <v>32.75859992753161</v>
       </c>
       <c r="G50" t="n">
-        <v>160.9031677246094</v>
+        <v>165.0220947265625</v>
       </c>
       <c r="H50" t="n">
-        <v>57.00967788696289</v>
+        <v>58.97706604003906</v>
       </c>
       <c r="I50" t="n">
-        <v>121.764045715332</v>
+        <v>118.5903930664062</v>
       </c>
       <c r="J50" t="n">
-        <v>126.6450958251953</v>
+        <v>125.9200973510742</v>
       </c>
     </row>
     <row r="51">
@@ -2073,16 +2073,16 @@
         <v>35.60454595063857</v>
       </c>
       <c r="G51" t="n">
-        <v>169.5130157470703</v>
+        <v>168.404052734375</v>
       </c>
       <c r="H51" t="n">
-        <v>55.69463729858398</v>
+        <v>55.78304290771484</v>
       </c>
       <c r="I51" t="n">
-        <v>151.6829833984375</v>
+        <v>151.2090759277344</v>
       </c>
       <c r="J51" t="n">
-        <v>126.7761993408203</v>
+        <v>122.4507675170898</v>
       </c>
     </row>
     <row r="52">
@@ -2105,16 +2105,16 @@
         <v>38.13811789539464</v>
       </c>
       <c r="G52" t="n">
-        <v>174.5154876708984</v>
+        <v>176.8798217773438</v>
       </c>
       <c r="H52" t="n">
-        <v>54.84718322753906</v>
+        <v>55.71947479248047</v>
       </c>
       <c r="I52" t="n">
-        <v>176.4033355712891</v>
+        <v>177.6861877441406</v>
       </c>
       <c r="J52" t="n">
-        <v>126.1392669677734</v>
+        <v>121.4752807617188</v>
       </c>
     </row>
     <row r="53">
@@ -2137,16 +2137,16 @@
         <v>39.1380055059179</v>
       </c>
       <c r="G53" t="n">
-        <v>187.0304107666016</v>
+        <v>183.3971099853516</v>
       </c>
       <c r="H53" t="n">
-        <v>60.91284942626953</v>
+        <v>57.20502471923828</v>
       </c>
       <c r="I53" t="n">
-        <v>225.8322448730469</v>
+        <v>230.3724517822266</v>
       </c>
       <c r="J53" t="n">
-        <v>125.8196716308594</v>
+        <v>121.8595504760742</v>
       </c>
     </row>
     <row r="54">
@@ -2169,16 +2169,16 @@
         <v>40.17007780104868</v>
       </c>
       <c r="G54" t="n">
-        <v>199.1808624267578</v>
+        <v>199.8622741699219</v>
       </c>
       <c r="H54" t="n">
-        <v>60.93319702148438</v>
+        <v>61.61745071411133</v>
       </c>
       <c r="I54" t="n">
-        <v>288.1661071777344</v>
+        <v>292.3958129882812</v>
       </c>
       <c r="J54" t="n">
-        <v>127.7896957397461</v>
+        <v>118.7660903930664</v>
       </c>
     </row>
     <row r="55">
@@ -2201,16 +2201,16 @@
         <v>40.31777520333784</v>
       </c>
       <c r="G55" t="n">
-        <v>208.4064636230469</v>
+        <v>211.8439483642578</v>
       </c>
       <c r="H55" t="n">
-        <v>60.87629318237305</v>
+        <v>61.71715927124023</v>
       </c>
       <c r="I55" t="n">
-        <v>343.974609375</v>
+        <v>337.5866394042969</v>
       </c>
       <c r="J55" t="n">
-        <v>140.7485656738281</v>
+        <v>130.0176849365234</v>
       </c>
     </row>
     <row r="56">
@@ -2233,16 +2233,16 @@
         <v>38.89328689858721</v>
       </c>
       <c r="G56" t="n">
-        <v>227.4288024902344</v>
+        <v>226.0331573486328</v>
       </c>
       <c r="H56" t="n">
-        <v>64.83397674560547</v>
+        <v>64.25822448730469</v>
       </c>
       <c r="I56" t="n">
-        <v>391.7401428222656</v>
+        <v>395.5137634277344</v>
       </c>
       <c r="J56" t="n">
-        <v>155.3560333251953</v>
+        <v>161.1677398681641</v>
       </c>
     </row>
     <row r="57">
@@ -2265,16 +2265,16 @@
         <v>36.03490394546852</v>
       </c>
       <c r="G57" t="n">
-        <v>271.2952270507812</v>
+        <v>268.876953125</v>
       </c>
       <c r="H57" t="n">
-        <v>86.47312927246094</v>
+        <v>83.87662506103516</v>
       </c>
       <c r="I57" t="n">
-        <v>403.3581237792969</v>
+        <v>400.4118347167969</v>
       </c>
       <c r="J57" t="n">
-        <v>193.6678009033203</v>
+        <v>203.0724029541016</v>
       </c>
     </row>
     <row r="58">
@@ -2297,16 +2297,16 @@
         <v>33.0417017672229</v>
       </c>
       <c r="G58" t="n">
-        <v>342.4889221191406</v>
+        <v>343.2109985351562</v>
       </c>
       <c r="H58" t="n">
-        <v>115.5745315551758</v>
+        <v>117.2090682983398</v>
       </c>
       <c r="I58" t="n">
-        <v>397.3973693847656</v>
+        <v>400.2284545898438</v>
       </c>
       <c r="J58" t="n">
-        <v>227.0475311279297</v>
+        <v>236.5142517089844</v>
       </c>
     </row>
     <row r="59">
@@ -2329,16 +2329,16 @@
         <v>43.98768298598323</v>
       </c>
       <c r="G59" t="n">
-        <v>176.6348266601562</v>
+        <v>173.9058685302734</v>
       </c>
       <c r="H59" t="n">
-        <v>60.02022171020508</v>
+        <v>57.64875793457031</v>
       </c>
       <c r="I59" t="n">
-        <v>115.6337509155273</v>
+        <v>117.7689819335938</v>
       </c>
       <c r="J59" t="n">
-        <v>126.6749954223633</v>
+        <v>139.9611968994141</v>
       </c>
     </row>
     <row r="60">
@@ -2361,16 +2361,16 @@
         <v>45.7006317110727</v>
       </c>
       <c r="G60" t="n">
-        <v>186.1289367675781</v>
+        <v>184.2041473388672</v>
       </c>
       <c r="H60" t="n">
-        <v>60.48526382446289</v>
+        <v>60.18131637573242</v>
       </c>
       <c r="I60" t="n">
-        <v>151.0547943115234</v>
+        <v>149.8686981201172</v>
       </c>
       <c r="J60" t="n">
-        <v>133.3187561035156</v>
+        <v>127.3840026855469</v>
       </c>
     </row>
     <row r="61">
@@ -2393,16 +2393,16 @@
         <v>46.67965674781412</v>
       </c>
       <c r="G61" t="n">
-        <v>194.8869171142578</v>
+        <v>197.2599029541016</v>
       </c>
       <c r="H61" t="n">
-        <v>63.25343322753906</v>
+        <v>65.73317718505859</v>
       </c>
       <c r="I61" t="n">
-        <v>201.4439849853516</v>
+        <v>197.8111877441406</v>
       </c>
       <c r="J61" t="n">
-        <v>129.7440032958984</v>
+        <v>124.9351272583008</v>
       </c>
     </row>
     <row r="62">
@@ -2425,16 +2425,16 @@
         <v>47.53914448671719</v>
       </c>
       <c r="G62" t="n">
-        <v>206.1235809326172</v>
+        <v>207.5868682861328</v>
       </c>
       <c r="H62" t="n">
-        <v>65.71555328369141</v>
+        <v>71.68706512451172</v>
       </c>
       <c r="I62" t="n">
-        <v>243.4985198974609</v>
+        <v>247.3363037109375</v>
       </c>
       <c r="J62" t="n">
-        <v>135.1009674072266</v>
+        <v>136.9089508056641</v>
       </c>
     </row>
     <row r="63">
@@ -2457,16 +2457,16 @@
         <v>47.07121651777462</v>
       </c>
       <c r="G63" t="n">
-        <v>222.6201629638672</v>
+        <v>220.3125457763672</v>
       </c>
       <c r="H63" t="n">
-        <v>70.35382843017578</v>
+        <v>68.53217315673828</v>
       </c>
       <c r="I63" t="n">
-        <v>318.1659851074219</v>
+        <v>322.0957946777344</v>
       </c>
       <c r="J63" t="n">
-        <v>137.3455047607422</v>
+        <v>145.4533386230469</v>
       </c>
     </row>
     <row r="64">
@@ -2489,16 +2489,16 @@
         <v>45.67156598130153</v>
       </c>
       <c r="G64" t="n">
-        <v>242.8789520263672</v>
+        <v>240.0746917724609</v>
       </c>
       <c r="H64" t="n">
-        <v>74.43870544433594</v>
+        <v>72.16489410400391</v>
       </c>
       <c r="I64" t="n">
-        <v>372.2238159179688</v>
+        <v>376.5995178222656</v>
       </c>
       <c r="J64" t="n">
-        <v>159.0616149902344</v>
+        <v>154.7747344970703</v>
       </c>
     </row>
     <row r="65">
@@ -2521,16 +2521,16 @@
         <v>42.51104340916319</v>
       </c>
       <c r="G65" t="n">
-        <v>276.8896179199219</v>
+        <v>281.3939819335938</v>
       </c>
       <c r="H65" t="n">
-        <v>83.67181396484375</v>
+        <v>90.35240173339844</v>
       </c>
       <c r="I65" t="n">
-        <v>398.5833740234375</v>
+        <v>393.7484741210938</v>
       </c>
       <c r="J65" t="n">
-        <v>193.4186096191406</v>
+        <v>193.1266479492188</v>
       </c>
     </row>
     <row r="66">
@@ -2553,16 +2553,16 @@
         <v>54.37577254606605</v>
       </c>
       <c r="G66" t="n">
-        <v>197.8959808349609</v>
+        <v>198.7372741699219</v>
       </c>
       <c r="H66" t="n">
-        <v>72.14685821533203</v>
+        <v>71.93898010253906</v>
       </c>
       <c r="I66" t="n">
-        <v>109.7955322265625</v>
+        <v>108.1383666992188</v>
       </c>
       <c r="J66" t="n">
-        <v>132.9255218505859</v>
+        <v>126.1202697753906</v>
       </c>
     </row>
     <row r="67">
@@ -2585,16 +2585,16 @@
         <v>55.07062752917076</v>
       </c>
       <c r="G67" t="n">
-        <v>207.1194152832031</v>
+        <v>208.4151916503906</v>
       </c>
       <c r="H67" t="n">
-        <v>73.87160491943359</v>
+        <v>71.12234497070312</v>
       </c>
       <c r="I67" t="n">
-        <v>154.2553253173828</v>
+        <v>159.5003967285156</v>
       </c>
       <c r="J67" t="n">
-        <v>128.3394165039062</v>
+        <v>145.4478149414062</v>
       </c>
     </row>
     <row r="68">
@@ -2617,16 +2617,16 @@
         <v>54.82432856758766</v>
       </c>
       <c r="G68" t="n">
-        <v>220.3422393798828</v>
+        <v>217.2136688232422</v>
       </c>
       <c r="H68" t="n">
-        <v>79.48954010009766</v>
+        <v>76.7850341796875</v>
       </c>
       <c r="I68" t="n">
-        <v>219.1385955810547</v>
+        <v>214.8410491943359</v>
       </c>
       <c r="J68" t="n">
-        <v>135.4891815185547</v>
+        <v>136.4175720214844</v>
       </c>
     </row>
     <row r="69">
@@ -2649,16 +2649,16 @@
         <v>54.18769809434324</v>
       </c>
       <c r="G69" t="n">
-        <v>237.9185180664062</v>
+        <v>237.5969543457031</v>
       </c>
       <c r="H69" t="n">
-        <v>87.444091796875</v>
+        <v>81.29430389404297</v>
       </c>
       <c r="I69" t="n">
-        <v>289.5146179199219</v>
+        <v>282.4862060546875</v>
       </c>
       <c r="J69" t="n">
-        <v>163.5497589111328</v>
+        <v>149.7420959472656</v>
       </c>
     </row>
     <row r="70">
@@ -2681,16 +2681,16 @@
         <v>51.347187815424</v>
       </c>
       <c r="G70" t="n">
-        <v>261.6987609863281</v>
+        <v>258.1413879394531</v>
       </c>
       <c r="H70" t="n">
-        <v>89.93715667724609</v>
+        <v>85.90751647949219</v>
       </c>
       <c r="I70" t="n">
-        <v>344.8820190429688</v>
+        <v>351.8117370605469</v>
       </c>
       <c r="J70" t="n">
-        <v>157.9957580566406</v>
+        <v>167.7597808837891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>